<commit_message>
Problem with material balances.
</commit_message>
<xml_diff>
--- a/Settings/Base/Ind30Pro39v1_BaseSectorClassification.xlsx
+++ b/Settings/Base/Ind30Pro39v1_BaseSectorClassification.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwieland\Github workspace\PIOLab\ConcordanceLibrary\LabelsAndCodes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwieland\Github workspace\PIOLab\Settings\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BaseProcesses" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="126">
   <si>
     <t>Iron ore</t>
   </si>
@@ -389,6 +389,24 @@
   </si>
   <si>
     <t>SteelOxygenBlownConverter</t>
+  </si>
+  <si>
+    <t>Type_2</t>
+  </si>
+  <si>
+    <t>Reduced iron</t>
+  </si>
+  <si>
+    <t>Liquid steel</t>
+  </si>
+  <si>
+    <t>Finished steel</t>
+  </si>
+  <si>
+    <t>Final product</t>
+  </si>
+  <si>
+    <t>Scrap</t>
   </si>
 </sst>
 </file>
@@ -728,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1207,19 +1225,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1230,10 +1249,13 @@
         <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1244,10 +1266,13 @@
         <v>92</v>
       </c>
       <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1257,11 +1282,14 @@
       <c r="C3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1272,10 +1300,13 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1285,11 +1316,14 @@
       <c r="C5" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1300,10 +1334,13 @@
         <v>71</v>
       </c>
       <c r="D6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1313,11 +1350,14 @@
       <c r="C7" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1328,10 +1368,13 @@
         <v>72</v>
       </c>
       <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1342,10 +1385,13 @@
         <v>72</v>
       </c>
       <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1356,10 +1402,13 @@
         <v>72</v>
       </c>
       <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1370,10 +1419,13 @@
         <v>72</v>
       </c>
       <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1383,11 +1435,14 @@
       <c r="C12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1397,11 +1452,14 @@
       <c r="C13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1411,11 +1469,14 @@
       <c r="C14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1425,11 +1486,14 @@
       <c r="C15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1439,11 +1503,14 @@
       <c r="C16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1453,11 +1520,14 @@
       <c r="C17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1467,11 +1537,14 @@
       <c r="C18" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1481,11 +1554,14 @@
       <c r="C19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1495,11 +1571,14 @@
       <c r="C20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1509,11 +1588,14 @@
       <c r="C21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1523,11 +1605,14 @@
       <c r="C22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1537,11 +1622,14 @@
       <c r="C23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1551,11 +1639,14 @@
       <c r="C24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1565,11 +1656,14 @@
       <c r="C25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1580,10 +1674,13 @@
         <v>73</v>
       </c>
       <c r="D26" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1593,11 +1690,14 @@
       <c r="C27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1608,10 +1708,13 @@
         <v>74</v>
       </c>
       <c r="D28" t="s">
+        <v>124</v>
+      </c>
+      <c r="E28" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1622,10 +1725,13 @@
         <v>74</v>
       </c>
       <c r="D29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1636,10 +1742,13 @@
         <v>74</v>
       </c>
       <c r="D30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1650,10 +1759,13 @@
         <v>74</v>
       </c>
       <c r="D31" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1664,10 +1776,13 @@
         <v>74</v>
       </c>
       <c r="D32" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1678,10 +1793,13 @@
         <v>74</v>
       </c>
       <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1692,10 +1810,13 @@
         <v>74</v>
       </c>
       <c r="D34" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1706,10 +1827,13 @@
         <v>74</v>
       </c>
       <c r="D35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1720,10 +1844,13 @@
         <v>74</v>
       </c>
       <c r="D36" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1734,10 +1861,13 @@
         <v>74</v>
       </c>
       <c r="D37" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1748,10 +1878,13 @@
         <v>75</v>
       </c>
       <c r="D38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1762,10 +1895,13 @@
         <v>75</v>
       </c>
       <c r="D39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1776,6 +1912,9 @@
         <v>75</v>
       </c>
       <c r="D40" t="s">
+        <v>125</v>
+      </c>
+      <c r="E40" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a new column with infos for aggregating the table for Sankeys.
</commit_message>
<xml_diff>
--- a/Settings/Base/Ind30Pro39v1_BaseSectorClassification.xlsx
+++ b/Settings/Base/Ind30Pro39v1_BaseSectorClassification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="BaseProcesses" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="129">
   <si>
     <t>Iron ore</t>
   </si>
@@ -407,6 +407,15 @@
   </si>
   <si>
     <t>Scrap</t>
+  </si>
+  <si>
+    <t>Other manufacturing products</t>
+  </si>
+  <si>
+    <t>Aggregate</t>
+  </si>
+  <si>
+    <t>Manufactruing n.e.c.</t>
   </si>
 </sst>
 </file>
@@ -466,7 +475,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -482,7 +491,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -744,19 +753,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="67.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -778,8 +787,11 @@
       <c r="G1" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -792,8 +804,11 @@
       <c r="D2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -806,8 +821,11 @@
       <c r="D3" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -820,8 +838,11 @@
       <c r="D4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -834,8 +855,11 @@
       <c r="D5" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -848,8 +872,11 @@
       <c r="D6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -862,8 +889,11 @@
       <c r="D7" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -876,8 +906,11 @@
       <c r="D8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -890,8 +923,11 @@
       <c r="D9" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -904,8 +940,11 @@
       <c r="D10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -918,8 +957,11 @@
       <c r="D11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -932,8 +974,11 @@
       <c r="D12" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -946,8 +991,11 @@
       <c r="D13" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -969,8 +1017,11 @@
       <c r="G14" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -983,8 +1034,11 @@
       <c r="D15" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -997,8 +1051,11 @@
       <c r="D16" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1014,8 +1071,11 @@
       <c r="E17" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1034,8 +1094,11 @@
       <c r="F18" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1048,8 +1111,11 @@
       <c r="D19" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1062,8 +1128,11 @@
       <c r="D20" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1076,8 +1145,11 @@
       <c r="D21" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1090,8 +1162,11 @@
       <c r="D22" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1104,8 +1179,11 @@
       <c r="D23" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1118,8 +1196,11 @@
       <c r="D24" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1132,8 +1213,11 @@
       <c r="D25" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1146,8 +1230,11 @@
       <c r="D26" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1160,8 +1247,11 @@
       <c r="D27" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1174,8 +1264,11 @@
       <c r="D28" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1188,8 +1281,11 @@
       <c r="D29" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1202,8 +1298,11 @@
       <c r="D30" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1215,6 +1314,9 @@
       </c>
       <c r="D31" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="H31" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1225,20 +1327,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1254,8 +1356,11 @@
       <c r="E1" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1271,8 +1376,11 @@
       <c r="E2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1288,8 +1396,11 @@
       <c r="E3" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1305,8 +1416,11 @@
       <c r="E4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1322,8 +1436,11 @@
       <c r="E5" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1339,8 +1456,11 @@
       <c r="E6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1356,8 +1476,11 @@
       <c r="E7" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1373,8 +1496,11 @@
       <c r="E8" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1390,8 +1516,11 @@
       <c r="E9" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1407,8 +1536,11 @@
       <c r="E10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1424,8 +1556,11 @@
       <c r="E11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1441,8 +1576,11 @@
       <c r="E12" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1458,8 +1596,11 @@
       <c r="E13" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1475,8 +1616,11 @@
       <c r="E14" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1492,8 +1636,11 @@
       <c r="E15" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1509,8 +1656,11 @@
       <c r="E16" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1526,8 +1676,11 @@
       <c r="E17" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1543,8 +1696,11 @@
       <c r="E18" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1560,8 +1716,11 @@
       <c r="E19" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1577,8 +1736,11 @@
       <c r="E20" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1594,8 +1756,11 @@
       <c r="E21" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1611,8 +1776,11 @@
       <c r="E22" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1628,8 +1796,11 @@
       <c r="E23" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1645,8 +1816,11 @@
       <c r="E24" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1662,8 +1836,11 @@
       <c r="E25" s="4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1679,8 +1856,11 @@
       <c r="E26" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1696,8 +1876,11 @@
       <c r="E27" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1713,8 +1896,11 @@
       <c r="E28" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1730,8 +1916,11 @@
       <c r="E29" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1747,8 +1936,11 @@
       <c r="E30" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1764,8 +1956,11 @@
       <c r="E31" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1781,8 +1976,11 @@
       <c r="E32" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1798,8 +1996,11 @@
       <c r="E33" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1815,8 +2016,11 @@
       <c r="E34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1832,8 +2036,11 @@
       <c r="E35" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1849,8 +2056,11 @@
       <c r="E36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1866,8 +2076,11 @@
       <c r="E37" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1883,8 +2096,11 @@
       <c r="E38" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1900,8 +2116,11 @@
       <c r="E39" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1916,6 +2135,9 @@
       </c>
       <c r="E40" t="s">
         <v>114</v>
+      </c>
+      <c r="F40" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1932,9 +2154,9 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1945,7 +2167,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1956,7 +2178,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1967,7 +2189,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1978,7 +2200,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1989,7 +2211,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2000,7 +2222,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2011,7 +2233,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2022,7 +2244,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2053,9 +2275,9 @@
       <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -2063,7 +2285,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2071,7 +2293,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2079,7 +2301,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2087,7 +2309,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2095,7 +2317,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2103,10 +2325,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
     </row>
   </sheetData>
@@ -2128,9 +2350,9 @@
       <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2249,7 +2471,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -2371,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -2493,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2615,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -2737,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -2859,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -2981,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -3103,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -3225,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -3347,7 +3569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -3469,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -3591,7 +3813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -3713,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -3835,7 +4057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -3957,7 +4179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -4079,7 +4301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -4201,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -4323,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -4445,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -4567,7 +4789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -4689,7 +4911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -4811,7 +5033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -4933,7 +5155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -5055,7 +5277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -5177,7 +5399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -5299,7 +5521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -5421,7 +5643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -5543,7 +5765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -5665,7 +5887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -5787,7 +6009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -5928,13 +6150,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>38</v>
       </c>
@@ -6026,7 +6248,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6121,7 +6343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6216,7 +6438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -6311,7 +6533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -6406,7 +6628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -6501,7 +6723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -6596,7 +6818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -6691,7 +6913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -6786,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -6881,7 +7103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -6976,7 +7198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -7071,7 +7293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -7166,7 +7388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -7261,7 +7483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -7356,7 +7578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -7451,7 +7673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -7546,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -7641,7 +7863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -7736,7 +7958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -7831,7 +8053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -7926,7 +8148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -8021,7 +8243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -8116,7 +8338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -8211,7 +8433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -8306,7 +8528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -8401,7 +8623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -8496,7 +8718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -8591,7 +8813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -8686,7 +8908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -8781,7 +9003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -8876,7 +9098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -8971,7 +9193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -9066,7 +9288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -9161,7 +9383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -9256,7 +9478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -9351,7 +9573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -9446,7 +9668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -9541,7 +9763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -9636,7 +9858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -9731,7 +9953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>86</v>
       </c>
@@ -9826,7 +10048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>87</v>
       </c>
@@ -9921,7 +10143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>88</v>
       </c>
@@ -10016,7 +10238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>85</v>
       </c>
@@ -10111,7 +10333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>89</v>
       </c>

</xml_diff>